<commit_message>
cập nhật file annresult
</commit_message>
<xml_diff>
--- a/Document/ANNTestResult.xlsx
+++ b/Document/ANNTestResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="7740"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>period = 1</t>
   </si>
@@ -43,13 +43,16 @@
   </si>
   <si>
     <t>VNM</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,7 +172,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -204,7 +206,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -380,20 +381,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -406,8 +409,20 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -423,8 +438,20 @@
       <c r="E3">
         <v>58.45</v>
       </c>
+      <c r="G3">
+        <v>65.47</v>
+      </c>
+      <c r="H3">
+        <v>55.85</v>
+      </c>
+      <c r="I3">
+        <v>54.78</v>
+      </c>
+      <c r="J3">
+        <v>36.47</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -437,8 +464,20 @@
       <c r="E4">
         <v>55.55</v>
       </c>
+      <c r="G4">
+        <v>56.98</v>
+      </c>
+      <c r="H4">
+        <v>51.35</v>
+      </c>
+      <c r="I4">
+        <v>52.72</v>
+      </c>
+      <c r="J4">
+        <v>33.33</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -454,8 +493,20 @@
       <c r="E5">
         <v>20.32</v>
       </c>
+      <c r="G5">
+        <v>65.42</v>
+      </c>
+      <c r="H5">
+        <v>55.08</v>
+      </c>
+      <c r="I5">
+        <v>45.7</v>
+      </c>
+      <c r="J5">
+        <v>36.26</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -471,8 +522,20 @@
       <c r="E6">
         <v>30.72</v>
       </c>
+      <c r="G6">
+        <v>61.08</v>
+      </c>
+      <c r="H6">
+        <v>54.35</v>
+      </c>
+      <c r="I6">
+        <v>38.79</v>
+      </c>
+      <c r="J6">
+        <v>29.61</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -484,6 +547,55 @@
       </c>
       <c r="E7">
         <v>34.950000000000003</v>
+      </c>
+      <c r="G7">
+        <v>57.75</v>
+      </c>
+      <c r="H7">
+        <v>58</v>
+      </c>
+      <c r="I7">
+        <v>44.78</v>
+      </c>
+      <c r="J7">
+        <v>34.950000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B3:B7)</f>
+        <v>49.77</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">AVERAGE(C3:C7)</f>
+        <v>38.545000000000002</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>40.42</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>39.998000000000005</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8" si="1">AVERAGE(G3:G7)</f>
+        <v>61.339999999999996</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8" si="2">AVERAGE(H3:H7)</f>
+        <v>54.926000000000002</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:J8" si="3">AVERAGE(I3:I7)</f>
+        <v>47.353999999999999</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>34.124000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -492,24 +604,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cập nhật sơ kết quả test, còn test tiếp
</commit_message>
<xml_diff>
--- a/Document/ANNTestResult.xlsx
+++ b/Document/ANNTestResult.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>period = 1</t>
   </si>
@@ -46,16 +46,48 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>SVM - Đổi chu kỳ cho Aroon = 10</t>
+  </si>
+  <si>
+    <t>K-SVMeans</t>
+  </si>
+  <si>
+    <t>K = 2, Aroon 5, Volume</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>K=2 Aroon = 5, No Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,8 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,9 +432,35 @@
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="1" spans="1:15">
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -421,8 +485,11 @@
       <c r="J2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -450,8 +517,11 @@
       <c r="J3">
         <v>36.47</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3">
+        <v>60.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -476,8 +546,11 @@
       <c r="J4">
         <v>33.33</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4">
+        <v>56.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -505,8 +578,11 @@
       <c r="J5">
         <v>36.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5">
+        <v>70.209999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -534,8 +610,11 @@
       <c r="J6">
         <v>29.61</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6">
+        <v>56.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -560,17 +639,20 @@
       <c r="J7">
         <v>34.950000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7">
+        <v>57.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <f>AVERAGE(B3:B7)</f>
         <v>49.77</v>
       </c>
-      <c r="C8">
-        <f t="shared" ref="C8:F8" si="0">AVERAGE(C3:C7)</f>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:E8" si="0">AVERAGE(C3:C7)</f>
         <v>38.545000000000002</v>
       </c>
       <c r="D8">
@@ -581,25 +663,143 @@
         <f t="shared" si="0"/>
         <v>39.998000000000005</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <f t="shared" ref="G8" si="1">AVERAGE(G3:G7)</f>
         <v>61.339999999999996</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <f t="shared" ref="H8" si="2">AVERAGE(H3:H7)</f>
         <v>54.926000000000002</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:J8" si="3">AVERAGE(I3:I7)</f>
+        <f t="shared" ref="I8:L8" si="3">AVERAGE(I3:I7)</f>
         <v>47.353999999999999</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
         <v>34.124000000000002</v>
       </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>60.42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>59.29</v>
+      </c>
+      <c r="C13" s="4">
+        <v>61.33</v>
+      </c>
+      <c r="E13">
+        <v>66.430000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>56.98</v>
+      </c>
+      <c r="C14">
+        <v>56.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>70.739999999999995</v>
+      </c>
+      <c r="C15">
+        <v>42.24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>46.48</v>
+      </c>
+      <c r="C16">
+        <v>41.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>58.62</v>
+      </c>
+      <c r="C17">
+        <v>54.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:C18" si="4">AVERAGE(B13:B17)</f>
+        <v>58.42199999999999</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="4"/>
+        <v>51.253999999999998</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>